<commit_message>
changed to sql storage instead of csv
</commit_message>
<xml_diff>
--- a/sentiment_history.xlsx
+++ b/sentiment_history.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jstef\source\repos\StockTrender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B435D06-EBFC-40E0-B277-B0504618277C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A831AC0-BD7E-4195-A3D1-5E1DD46E572B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="4" xr2:uid="{CCF0F0B7-F616-44D9-980B-0193A0B0328A}"/>
   </bookViews>
   <sheets>
-    <sheet name="DOW News" sheetId="10" r:id="rId1"/>
-    <sheet name="DOW Twitter" sheetId="11" r:id="rId2"/>
-    <sheet name="NASDAQ Twitter" sheetId="13" r:id="rId3"/>
-    <sheet name="NASDAQ News" sheetId="9" r:id="rId4"/>
-    <sheet name="Graphs" sheetId="14" r:id="rId5"/>
+    <sheet name="DOW_news" sheetId="10" r:id="rId1"/>
+    <sheet name="DOW_twitter" sheetId="11" r:id="rId2"/>
+    <sheet name="NASDAQ_twitter" sheetId="13" r:id="rId3"/>
+    <sheet name="NASDAQ_news" sheetId="9" r:id="rId4"/>
+    <sheet name="Data Analysis" sheetId="14" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'NASDAQ News'!$A$1:$CZ$3</definedName>
-    <definedName name="ExternalData_2" localSheetId="0" hidden="1">'DOW News'!$A$1:$AE$3</definedName>
-    <definedName name="ExternalData_2" localSheetId="1" hidden="1">'DOW Twitter'!$A$1:$AE$3</definedName>
-    <definedName name="ExternalData_2" localSheetId="2" hidden="1">'NASDAQ Twitter'!$A$1:$CZ$3</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">NASDAQ_news!$A$1:$CZ$3</definedName>
+    <definedName name="ExternalData_2" localSheetId="0" hidden="1">DOW_news!$A$1:$AE$3</definedName>
+    <definedName name="ExternalData_2" localSheetId="1" hidden="1">DOW_twitter!$A$1:$AE$3</definedName>
+    <definedName name="ExternalData_2" localSheetId="2" hidden="1">NASDAQ_twitter!$A$1:$CZ$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -450,6 +450,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="174" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -479,9 +482,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1748,9 +1752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17DD3E9-CAC8-4886-979E-20F43E6EC5CE}">
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4152,7 +4154,17 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2">
+        <f>DOW_news!A$2</f>
+        <v>43526</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>